<commit_message>
Incorporo nuevos datos hasta diciembre de 2025
</commit_message>
<xml_diff>
--- a/DATOS/IPC ORIGINAL/IPC_2002_2025.xlsx
+++ b/DATOS/IPC ORIGINAL/IPC_2002_2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lorie\Desktop\TRABAJO\MICRODATOS\IPC\SUBGRUPOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lorie\Desktop\TRABAJO\CGT\Análisis de coyuntura económica\IPC\Nuevo calculo de IPC alternativo para inquilinos\reponderacionIPC_2\DATOS\IPC ORIGINAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="331">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -998,6 +998,21 @@
   <si>
     <t>2025M07</t>
   </si>
+  <si>
+    <t>2025M08</t>
+  </si>
+  <si>
+    <t>2025M09</t>
+  </si>
+  <si>
+    <t>2025M10</t>
+  </si>
+  <si>
+    <t>2025M11</t>
+  </si>
+  <si>
+    <t>2025M12</t>
+  </si>
 </sst>
 </file>
 
@@ -1379,10 +1394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:JX43"/>
+  <dimension ref="A1:KC43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="JQ1" workbookViewId="0">
-      <selection activeCell="JY1" sqref="JY1"/>
+    <sheetView tabSelected="1" topLeftCell="JS1" workbookViewId="0">
+      <selection activeCell="KH12" sqref="KH12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1391,7 +1406,7 @@
     <col min="2" max="282" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2244,8 +2259,23 @@
       <c r="JX1" s="2" t="s">
         <v>325</v>
       </c>
+      <c r="JY1" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="JZ1" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="KA1" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="KB1" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="KC1" s="2" t="s">
+        <v>330</v>
+      </c>
     </row>
-    <row r="2" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>282</v>
       </c>
@@ -3098,8 +3128,23 @@
       <c r="JX2" s="6">
         <v>118.777</v>
       </c>
+      <c r="JY2" s="6">
+        <v>118.824</v>
+      </c>
+      <c r="JZ2" s="6">
+        <v>118.485</v>
+      </c>
+      <c r="KA2" s="6">
+        <v>119.301</v>
+      </c>
+      <c r="KB2" s="6">
+        <v>119.532</v>
+      </c>
+      <c r="KC2" s="6">
+        <v>119.94199999999999</v>
+      </c>
     </row>
-    <row r="3" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>283</v>
       </c>
@@ -3952,8 +3997,23 @@
       <c r="JX3" s="6">
         <v>132.16200000000001</v>
       </c>
+      <c r="JY3" s="6">
+        <v>131.02099999999999</v>
+      </c>
+      <c r="JZ3" s="6">
+        <v>130.828</v>
+      </c>
+      <c r="KA3" s="6">
+        <v>132.786</v>
+      </c>
+      <c r="KB3" s="6">
+        <v>133.24199999999999</v>
+      </c>
+      <c r="KC3" s="6">
+        <v>133.51</v>
+      </c>
     </row>
-    <row r="4" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>284</v>
       </c>
@@ -4806,8 +4866,23 @@
       <c r="JX4" s="6">
         <v>134.834</v>
       </c>
+      <c r="JY4" s="6">
+        <v>135.09899999999999</v>
+      </c>
+      <c r="JZ4" s="6">
+        <v>134.96199999999999</v>
+      </c>
+      <c r="KA4" s="6">
+        <v>135.92599999999999</v>
+      </c>
+      <c r="KB4" s="6">
+        <v>136.096</v>
+      </c>
+      <c r="KC4" s="6">
+        <v>136.27500000000001</v>
+      </c>
     </row>
-    <row r="5" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>285</v>
       </c>
@@ -5660,8 +5735,23 @@
       <c r="JX5" s="6">
         <v>118.724</v>
       </c>
+      <c r="JY5" s="6">
+        <v>118.64</v>
+      </c>
+      <c r="JZ5" s="6">
+        <v>119.129</v>
+      </c>
+      <c r="KA5" s="6">
+        <v>119.386</v>
+      </c>
+      <c r="KB5" s="6">
+        <v>119.38</v>
+      </c>
+      <c r="KC5" s="6">
+        <v>117.14100000000001</v>
+      </c>
     </row>
-    <row r="6" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>286</v>
       </c>
@@ -6514,8 +6604,23 @@
       <c r="JX6" s="6">
         <v>122.801</v>
       </c>
+      <c r="JY6" s="6">
+        <v>122.81699999999999</v>
+      </c>
+      <c r="JZ6" s="6">
+        <v>122.818</v>
+      </c>
+      <c r="KA6" s="6">
+        <v>122.821</v>
+      </c>
+      <c r="KB6" s="6">
+        <v>123.232</v>
+      </c>
+      <c r="KC6" s="6">
+        <v>126.431</v>
+      </c>
     </row>
-    <row r="7" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>287</v>
       </c>
@@ -7368,8 +7473,23 @@
       <c r="JX7" s="6">
         <v>99.662000000000006</v>
       </c>
+      <c r="JY7" s="6">
+        <v>98.683999999999997</v>
+      </c>
+      <c r="JZ7" s="6">
+        <v>101.349</v>
+      </c>
+      <c r="KA7" s="6">
+        <v>110.83</v>
+      </c>
+      <c r="KB7" s="6">
+        <v>115.42700000000001</v>
+      </c>
+      <c r="KC7" s="6">
+        <v>114.23</v>
+      </c>
     </row>
-    <row r="8" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>288</v>
       </c>
@@ -8222,8 +8342,23 @@
       <c r="JX8" s="6">
         <v>103.86499999999999</v>
       </c>
+      <c r="JY8" s="6">
+        <v>102.81399999999999</v>
+      </c>
+      <c r="JZ8" s="6">
+        <v>104.626</v>
+      </c>
+      <c r="KA8" s="6">
+        <v>109.45099999999999</v>
+      </c>
+      <c r="KB8" s="6">
+        <v>113.102</v>
+      </c>
+      <c r="KC8" s="6">
+        <v>112.81100000000001</v>
+      </c>
     </row>
-    <row r="9" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>289</v>
       </c>
@@ -9076,8 +9211,23 @@
       <c r="JX9" s="6">
         <v>108.39700000000001</v>
       </c>
+      <c r="JY9" s="6">
+        <v>108.545</v>
+      </c>
+      <c r="JZ9" s="6">
+        <v>108.759</v>
+      </c>
+      <c r="KA9" s="6">
+        <v>108.96599999999999</v>
+      </c>
+      <c r="KB9" s="6">
+        <v>109.172</v>
+      </c>
+      <c r="KC9" s="6">
+        <v>109.364</v>
+      </c>
     </row>
-    <row r="10" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>290</v>
       </c>
@@ -9930,8 +10080,23 @@
       <c r="JX10" s="6">
         <v>119.158</v>
       </c>
+      <c r="JY10" s="6">
+        <v>119.28100000000001</v>
+      </c>
+      <c r="JZ10" s="6">
+        <v>119.571</v>
+      </c>
+      <c r="KA10" s="6">
+        <v>119.834</v>
+      </c>
+      <c r="KB10" s="6">
+        <v>120.096</v>
+      </c>
+      <c r="KC10" s="6">
+        <v>120.245</v>
+      </c>
     </row>
-    <row r="11" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>291</v>
       </c>
@@ -10784,8 +10949,23 @@
       <c r="JX11" s="6">
         <v>110.301</v>
       </c>
+      <c r="JY11" s="6">
+        <v>110.44799999999999</v>
+      </c>
+      <c r="JZ11" s="6">
+        <v>112.381</v>
+      </c>
+      <c r="KA11" s="6">
+        <v>112.648</v>
+      </c>
+      <c r="KB11" s="6">
+        <v>112.673</v>
+      </c>
+      <c r="KC11" s="6">
+        <v>112.83799999999999</v>
+      </c>
     </row>
-    <row r="12" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>292</v>
       </c>
@@ -11638,8 +11818,23 @@
       <c r="JX12" s="6">
         <v>110.43899999999999</v>
       </c>
+      <c r="JY12" s="6">
+        <v>110.15900000000001</v>
+      </c>
+      <c r="JZ12" s="6">
+        <v>109.907</v>
+      </c>
+      <c r="KA12" s="6">
+        <v>112.161</v>
+      </c>
+      <c r="KB12" s="6">
+        <v>111.45099999999999</v>
+      </c>
+      <c r="KC12" s="6">
+        <v>112.77500000000001</v>
+      </c>
     </row>
-    <row r="13" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>293</v>
       </c>
@@ -12492,8 +12687,23 @@
       <c r="JX13" s="6">
         <v>113.59099999999999</v>
       </c>
+      <c r="JY13" s="6">
+        <v>113.449</v>
+      </c>
+      <c r="JZ13" s="6">
+        <v>113.97</v>
+      </c>
+      <c r="KA13" s="6">
+        <v>114.535</v>
+      </c>
+      <c r="KB13" s="6">
+        <v>114.971</v>
+      </c>
+      <c r="KC13" s="6">
+        <v>114.827</v>
+      </c>
     </row>
-    <row r="14" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>294</v>
       </c>
@@ -13346,8 +13556,23 @@
       <c r="JX14" s="6">
         <v>102.861</v>
       </c>
+      <c r="JY14" s="6">
+        <v>102.417</v>
+      </c>
+      <c r="JZ14" s="6">
+        <v>103.206</v>
+      </c>
+      <c r="KA14" s="6">
+        <v>104.468</v>
+      </c>
+      <c r="KB14" s="6">
+        <v>105.80200000000001</v>
+      </c>
+      <c r="KC14" s="6">
+        <v>106.289</v>
+      </c>
     </row>
-    <row r="15" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>295</v>
       </c>
@@ -14200,8 +14425,23 @@
       <c r="JX15" s="6">
         <v>104.214</v>
       </c>
+      <c r="JY15" s="6">
+        <v>104.291</v>
+      </c>
+      <c r="JZ15" s="6">
+        <v>104.423</v>
+      </c>
+      <c r="KA15" s="6">
+        <v>104.648</v>
+      </c>
+      <c r="KB15" s="6">
+        <v>104.506</v>
+      </c>
+      <c r="KC15" s="6">
+        <v>104.05</v>
+      </c>
     </row>
-    <row r="16" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>296</v>
       </c>
@@ -15054,8 +15294,23 @@
       <c r="JX16" s="6">
         <v>116.595</v>
       </c>
+      <c r="JY16" s="6">
+        <v>116.303</v>
+      </c>
+      <c r="JZ16" s="6">
+        <v>116.285</v>
+      </c>
+      <c r="KA16" s="6">
+        <v>116.437</v>
+      </c>
+      <c r="KB16" s="6">
+        <v>116.749</v>
+      </c>
+      <c r="KC16" s="6">
+        <v>116.679</v>
+      </c>
     </row>
-    <row r="17" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>297</v>
       </c>
@@ -15908,8 +16163,23 @@
       <c r="JX17" s="6">
         <v>105.389</v>
       </c>
+      <c r="JY17" s="6">
+        <v>105.009</v>
+      </c>
+      <c r="JZ17" s="6">
+        <v>105.46899999999999</v>
+      </c>
+      <c r="KA17" s="6">
+        <v>105.476</v>
+      </c>
+      <c r="KB17" s="6">
+        <v>105.696</v>
+      </c>
+      <c r="KC17" s="6">
+        <v>105.73399999999999</v>
+      </c>
     </row>
-    <row r="18" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>298</v>
       </c>
@@ -16762,8 +17032,23 @@
       <c r="JX18" s="6">
         <v>118.121</v>
       </c>
+      <c r="JY18" s="6">
+        <v>118.321</v>
+      </c>
+      <c r="JZ18" s="6">
+        <v>118.114</v>
+      </c>
+      <c r="KA18" s="6">
+        <v>118.446</v>
+      </c>
+      <c r="KB18" s="6">
+        <v>118.681</v>
+      </c>
+      <c r="KC18" s="6">
+        <v>118.587</v>
+      </c>
     </row>
-    <row r="19" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>299</v>
       </c>
@@ -17616,8 +17901,23 @@
       <c r="JX19" s="6">
         <v>103.938</v>
       </c>
+      <c r="JY19" s="6">
+        <v>103.842</v>
+      </c>
+      <c r="JZ19" s="6">
+        <v>103.907</v>
+      </c>
+      <c r="KA19" s="6">
+        <v>104.06</v>
+      </c>
+      <c r="KB19" s="6">
+        <v>104.188</v>
+      </c>
+      <c r="KC19" s="6">
+        <v>104.348</v>
+      </c>
     </row>
-    <row r="20" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>300</v>
       </c>
@@ -18470,8 +18770,23 @@
       <c r="JX20" s="6">
         <v>112.73699999999999</v>
       </c>
+      <c r="JY20" s="6">
+        <v>112.83199999999999</v>
+      </c>
+      <c r="JZ20" s="6">
+        <v>113.008</v>
+      </c>
+      <c r="KA20" s="6">
+        <v>113.238</v>
+      </c>
+      <c r="KB20" s="6">
+        <v>113.35299999999999</v>
+      </c>
+      <c r="KC20" s="6">
+        <v>113.57</v>
+      </c>
     </row>
-    <row r="21" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>301</v>
       </c>
@@ -19324,8 +19639,23 @@
       <c r="JX21" s="6">
         <v>107.941</v>
       </c>
+      <c r="JY21" s="6">
+        <v>108.036</v>
+      </c>
+      <c r="JZ21" s="6">
+        <v>108.02200000000001</v>
+      </c>
+      <c r="KA21" s="6">
+        <v>108.087</v>
+      </c>
+      <c r="KB21" s="6">
+        <v>108.152</v>
+      </c>
+      <c r="KC21" s="6">
+        <v>108.265</v>
+      </c>
     </row>
-    <row r="22" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>302</v>
       </c>
@@ -20178,8 +20508,23 @@
       <c r="JX22" s="6">
         <v>118.72799999999999</v>
       </c>
+      <c r="JY22" s="6">
+        <v>119.02</v>
+      </c>
+      <c r="JZ22" s="6">
+        <v>119.065</v>
+      </c>
+      <c r="KA22" s="6">
+        <v>118.843</v>
+      </c>
+      <c r="KB22" s="6">
+        <v>119.374</v>
+      </c>
+      <c r="KC22" s="6">
+        <v>119.604</v>
+      </c>
     </row>
-    <row r="23" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>303</v>
       </c>
@@ -21032,8 +21377,23 @@
       <c r="JX23" s="6">
         <v>113.432</v>
       </c>
+      <c r="JY23" s="6">
+        <v>112.998</v>
+      </c>
+      <c r="JZ23" s="6">
+        <v>112.99</v>
+      </c>
+      <c r="KA23" s="6">
+        <v>112.788</v>
+      </c>
+      <c r="KB23" s="6">
+        <v>113.997</v>
+      </c>
+      <c r="KC23" s="6">
+        <v>113.11</v>
+      </c>
     </row>
-    <row r="24" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>304</v>
       </c>
@@ -21886,8 +22246,23 @@
       <c r="JX24" s="6">
         <v>94.606999999999999</v>
       </c>
+      <c r="JY24" s="6">
+        <v>97.406000000000006</v>
+      </c>
+      <c r="JZ24" s="6">
+        <v>91.786000000000001</v>
+      </c>
+      <c r="KA24" s="6">
+        <v>95.278999999999996</v>
+      </c>
+      <c r="KB24" s="6">
+        <v>93.177000000000007</v>
+      </c>
+      <c r="KC24" s="6">
+        <v>95.555999999999997</v>
+      </c>
     </row>
-    <row r="25" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>305</v>
       </c>
@@ -22740,8 +23115,23 @@
       <c r="JX25" s="6">
         <v>71.340999999999994</v>
       </c>
+      <c r="JY25" s="6">
+        <v>72.132999999999996</v>
+      </c>
+      <c r="JZ25" s="6">
+        <v>71.620999999999995</v>
+      </c>
+      <c r="KA25" s="6">
+        <v>73.53</v>
+      </c>
+      <c r="KB25" s="6">
+        <v>72.489999999999995</v>
+      </c>
+      <c r="KC25" s="6">
+        <v>71.305000000000007</v>
+      </c>
     </row>
-    <row r="26" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>306</v>
       </c>
@@ -23594,8 +23984,23 @@
       <c r="JX26" s="6">
         <v>106.288</v>
       </c>
+      <c r="JY26" s="6">
+        <v>106.288</v>
+      </c>
+      <c r="JZ26" s="6">
+        <v>106.288</v>
+      </c>
+      <c r="KA26" s="6">
+        <v>106.006</v>
+      </c>
+      <c r="KB26" s="6">
+        <v>106.006</v>
+      </c>
+      <c r="KC26" s="6">
+        <v>106.006</v>
+      </c>
     </row>
-    <row r="27" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>307</v>
       </c>
@@ -24448,8 +24853,23 @@
       <c r="JX27" s="6">
         <v>84.221999999999994</v>
       </c>
+      <c r="JY27" s="6">
+        <v>84.435000000000002</v>
+      </c>
+      <c r="JZ27" s="6">
+        <v>84.203000000000003</v>
+      </c>
+      <c r="KA27" s="6">
+        <v>84.905000000000001</v>
+      </c>
+      <c r="KB27" s="6">
+        <v>84.313999999999993</v>
+      </c>
+      <c r="KC27" s="6">
+        <v>84.503</v>
+      </c>
     </row>
-    <row r="28" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>308</v>
       </c>
@@ -25302,8 +25722,23 @@
       <c r="JX28" s="6">
         <v>110.25</v>
       </c>
+      <c r="JY28" s="6">
+        <v>110.29600000000001</v>
+      </c>
+      <c r="JZ28" s="6">
+        <v>110.39100000000001</v>
+      </c>
+      <c r="KA28" s="6">
+        <v>111.316</v>
+      </c>
+      <c r="KB28" s="6">
+        <v>111.375</v>
+      </c>
+      <c r="KC28" s="6">
+        <v>110.749</v>
+      </c>
     </row>
-    <row r="29" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>309</v>
       </c>
@@ -26156,8 +26591,23 @@
       <c r="JX29" s="6">
         <v>108.047</v>
       </c>
+      <c r="JY29" s="6">
+        <v>108.02</v>
+      </c>
+      <c r="JZ29" s="6">
+        <v>108.19</v>
+      </c>
+      <c r="KA29" s="6">
+        <v>108.42400000000001</v>
+      </c>
+      <c r="KB29" s="6">
+        <v>108.738</v>
+      </c>
+      <c r="KC29" s="6">
+        <v>108.53700000000001</v>
+      </c>
     </row>
-    <row r="30" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>310</v>
       </c>
@@ -27010,8 +27460,23 @@
       <c r="JX30" s="6">
         <v>114.09</v>
       </c>
+      <c r="JY30" s="6">
+        <v>114.209</v>
+      </c>
+      <c r="JZ30" s="6">
+        <v>114.401</v>
+      </c>
+      <c r="KA30" s="6">
+        <v>114.806</v>
+      </c>
+      <c r="KB30" s="6">
+        <v>114.902</v>
+      </c>
+      <c r="KC30" s="6">
+        <v>115.127</v>
+      </c>
     </row>
-    <row r="31" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>311</v>
       </c>
@@ -27864,8 +28329,23 @@
       <c r="JX31" s="6">
         <v>161.43600000000001</v>
       </c>
+      <c r="JY31" s="6">
+        <v>171.51900000000001</v>
+      </c>
+      <c r="JZ31" s="6">
+        <v>141.60499999999999</v>
+      </c>
+      <c r="KA31" s="6">
+        <v>133.85499999999999</v>
+      </c>
+      <c r="KB31" s="6">
+        <v>130.648</v>
+      </c>
+      <c r="KC31" s="6">
+        <v>150.15899999999999</v>
+      </c>
     </row>
-    <row r="32" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>312</v>
       </c>
@@ -28718,8 +29198,23 @@
       <c r="JX32" s="6">
         <v>109.265</v>
       </c>
+      <c r="JY32" s="6">
+        <v>109.265</v>
+      </c>
+      <c r="JZ32" s="6">
+        <v>113.486</v>
+      </c>
+      <c r="KA32" s="6">
+        <v>113.64700000000001</v>
+      </c>
+      <c r="KB32" s="6">
+        <v>113.71899999999999</v>
+      </c>
+      <c r="KC32" s="6">
+        <v>113.721</v>
+      </c>
     </row>
-    <row r="33" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>313</v>
       </c>
@@ -29572,8 +30067,23 @@
       <c r="JX33" s="6">
         <v>113.214</v>
       </c>
+      <c r="JY33" s="6">
+        <v>113.214</v>
+      </c>
+      <c r="JZ33" s="6">
+        <v>117.053</v>
+      </c>
+      <c r="KA33" s="6">
+        <v>117.271</v>
+      </c>
+      <c r="KB33" s="6">
+        <v>117.316</v>
+      </c>
+      <c r="KC33" s="6">
+        <v>117.316</v>
+      </c>
     </row>
-    <row r="34" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>314</v>
       </c>
@@ -30426,8 +30936,23 @@
       <c r="JX34" s="6">
         <v>105.06</v>
       </c>
+      <c r="JY34" s="6">
+        <v>105.06</v>
+      </c>
+      <c r="JZ34" s="6">
+        <v>105.06</v>
+      </c>
+      <c r="KA34" s="6">
+        <v>106.413</v>
+      </c>
+      <c r="KB34" s="6">
+        <v>106.413</v>
+      </c>
+      <c r="KC34" s="6">
+        <v>106.413</v>
+      </c>
     </row>
-    <row r="35" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>315</v>
       </c>
@@ -31280,8 +31805,23 @@
       <c r="JX35" s="6">
         <v>108.358</v>
       </c>
+      <c r="JY35" s="6">
+        <v>108.44</v>
+      </c>
+      <c r="JZ35" s="6">
+        <v>109.048</v>
+      </c>
+      <c r="KA35" s="6">
+        <v>109.779</v>
+      </c>
+      <c r="KB35" s="6">
+        <v>110.47</v>
+      </c>
+      <c r="KC35" s="6">
+        <v>110.57299999999999</v>
+      </c>
     </row>
-    <row r="36" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>316</v>
       </c>
@@ -32134,8 +32674,23 @@
       <c r="JX36" s="6">
         <v>122.69799999999999</v>
       </c>
+      <c r="JY36" s="6">
+        <v>123.001</v>
+      </c>
+      <c r="JZ36" s="6">
+        <v>123.399</v>
+      </c>
+      <c r="KA36" s="6">
+        <v>123.82599999999999</v>
+      </c>
+      <c r="KB36" s="6">
+        <v>124.151</v>
+      </c>
+      <c r="KC36" s="6">
+        <v>124.577</v>
+      </c>
     </row>
-    <row r="37" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>317</v>
       </c>
@@ -32988,8 +33543,23 @@
       <c r="JX37" s="6">
         <v>160.643</v>
       </c>
+      <c r="JY37" s="6">
+        <v>162.02699999999999</v>
+      </c>
+      <c r="JZ37" s="6">
+        <v>161.33500000000001</v>
+      </c>
+      <c r="KA37" s="6">
+        <v>154.238</v>
+      </c>
+      <c r="KB37" s="6">
+        <v>141.995</v>
+      </c>
+      <c r="KC37" s="6">
+        <v>139.40100000000001</v>
+      </c>
     </row>
-    <row r="38" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>318</v>
       </c>
@@ -33842,8 +34412,23 @@
       <c r="JX38" s="6">
         <v>113.95</v>
       </c>
+      <c r="JY38" s="6">
+        <v>114.44499999999999</v>
+      </c>
+      <c r="JZ38" s="6">
+        <v>114.26300000000001</v>
+      </c>
+      <c r="KA38" s="6">
+        <v>114.369</v>
+      </c>
+      <c r="KB38" s="6">
+        <v>114.57299999999999</v>
+      </c>
+      <c r="KC38" s="6">
+        <v>114.57299999999999</v>
+      </c>
     </row>
-    <row r="39" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>319</v>
       </c>
@@ -34696,8 +35281,23 @@
       <c r="JX39" s="6">
         <v>119.081</v>
       </c>
+      <c r="JY39" s="6">
+        <v>118.985</v>
+      </c>
+      <c r="JZ39" s="6">
+        <v>120.04300000000001</v>
+      </c>
+      <c r="KA39" s="6">
+        <v>123.268</v>
+      </c>
+      <c r="KB39" s="6">
+        <v>126.492</v>
+      </c>
+      <c r="KC39" s="6">
+        <v>127.911</v>
+      </c>
     </row>
-    <row r="40" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>320</v>
       </c>
@@ -35550,8 +36150,23 @@
       <c r="JX40" s="6">
         <v>119.78400000000001</v>
       </c>
+      <c r="JY40" s="6">
+        <v>119.797</v>
+      </c>
+      <c r="JZ40" s="6">
+        <v>119.876</v>
+      </c>
+      <c r="KA40" s="6">
+        <v>119.905</v>
+      </c>
+      <c r="KB40" s="6">
+        <v>119.917</v>
+      </c>
+      <c r="KC40" s="6">
+        <v>120.021</v>
+      </c>
     </row>
-    <row r="41" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>321</v>
       </c>
@@ -36404,8 +37019,23 @@
       <c r="JX41" s="6">
         <v>130.16900000000001</v>
       </c>
+      <c r="JY41" s="6">
+        <v>130.16900000000001</v>
+      </c>
+      <c r="JZ41" s="6">
+        <v>130.16900000000001</v>
+      </c>
+      <c r="KA41" s="6">
+        <v>130.16900000000001</v>
+      </c>
+      <c r="KB41" s="6">
+        <v>130.16900000000001</v>
+      </c>
+      <c r="KC41" s="6">
+        <v>130.16900000000001</v>
+      </c>
     </row>
-    <row r="42" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>322</v>
       </c>
@@ -37258,8 +37888,23 @@
       <c r="JX42" s="6">
         <v>109.723</v>
       </c>
+      <c r="JY42" s="6">
+        <v>109.723</v>
+      </c>
+      <c r="JZ42" s="6">
+        <v>109.723</v>
+      </c>
+      <c r="KA42" s="6">
+        <v>109.723</v>
+      </c>
+      <c r="KB42" s="6">
+        <v>109.723</v>
+      </c>
+      <c r="KC42" s="6">
+        <v>109.723</v>
+      </c>
     </row>
-    <row r="43" spans="1:284" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:289" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>323</v>
       </c>
@@ -38111,6 +38756,21 @@
       </c>
       <c r="JX43" s="6">
         <v>106.196</v>
+      </c>
+      <c r="JY43" s="6">
+        <v>106.18899999999999</v>
+      </c>
+      <c r="JZ43" s="6">
+        <v>106.255</v>
+      </c>
+      <c r="KA43" s="6">
+        <v>106.328</v>
+      </c>
+      <c r="KB43" s="6">
+        <v>106.352</v>
+      </c>
+      <c r="KC43" s="6">
+        <v>106.357</v>
       </c>
     </row>
   </sheetData>

</xml_diff>